<commit_message>
Updated carbon tax rate and fuel use data
</commit_message>
<xml_diff>
--- a/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
+++ b/InputData/fuels/BCTR/BAU Carbon Tax Rate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anaxolt/Google Drive/2021/D.Development/TARGET_eps-us-3.2.1/InputData/fuels/BCTR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssy02\Desktop\eps-mexico-3.3.1.1\eps-mexico-3.3.1.1\InputData\fuels\BCTR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B93C6C-45F4-464E-8ED4-9465B14F521C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E08AF33-8C79-4BA0-8795-778D2CB26A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="500" windowWidth="23960" windowHeight="16500" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A875A243-FD0C-4B21-82AE-BAE80D34FF17}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -210,9 +210,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -250,7 +250,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -356,7 +356,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -498,7 +498,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -508,18 +508,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49357908-BC85-41CC-9D98-173369A13AF6}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -527,30 +527,30 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="5">
         <v>2014</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -562,7 +562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -573,7 +573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -584,21 +584,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
   </sheetData>
@@ -618,16 +618,16 @@
   </sheetPr>
   <dimension ref="A1:AG9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:AG5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -728,140 +728,108 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="10">
-        <f>About!$B$10</f>
-        <v>0.99</v>
-      </c>
-      <c r="C2">
-        <f t="shared" ref="C2:AG5" si="0">B2</f>
-        <v>0.99</v>
-      </c>
-      <c r="D2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="E2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="F2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="G2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="H2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="I2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="J2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="K2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="L2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="M2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="N2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="O2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="P2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="Q2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="R2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="S2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="T2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="U2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="V2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="W2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="X2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="Y2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="Z2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AA2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AB2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AC2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AD2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AE2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AF2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AG2">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+        <v>3.5</v>
+      </c>
+      <c r="C2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="D2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="E2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="F2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="G2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="H2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="I2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="J2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="K2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="L2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="M2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="N2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="O2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="P2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="R2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="S2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="T2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="U2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="V2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="W2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="X2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="Y2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="Z2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AA2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AB2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AC2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AD2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AE2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AF2" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AG2" s="10">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -962,406 +930,310 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="10">
-        <f>About!$B$10</f>
-        <v>0.99</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="N4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="O4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="P4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="Q4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="R4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="S4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="T4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="U4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="V4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="W4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="X4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="Y4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="Z4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AA4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AB4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AC4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AD4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AE4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AF4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AG4">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+        <v>3.5</v>
+      </c>
+      <c r="C4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="D4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="E4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="F4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="G4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="H4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="I4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="J4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="K4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="L4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="M4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="N4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="O4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="P4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="R4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="S4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="T4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="U4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="V4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="W4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="X4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="Y4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="Z4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AA4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AB4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AC4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AD4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AE4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AF4" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AG4" s="10">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="10">
-        <f>About!$B$10</f>
-        <v>0.99</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="R5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="S5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="T5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="U5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="V5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="W5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="X5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="Y5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="Z5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AA5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AB5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AC5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AD5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AE5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AF5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-      <c r="AG5">
-        <f t="shared" si="0"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+        <v>3.5</v>
+      </c>
+      <c r="C5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="D5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="E5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="F5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="G5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="H5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="I5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="J5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="K5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="L5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="M5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="N5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="O5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="P5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="R5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="S5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="T5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="U5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="V5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="W5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="X5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="Y5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="Z5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AA5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AB5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AC5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AD5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AE5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AF5" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AG5" s="10">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="10">
-        <f>About!$B$10</f>
-        <v>0.99</v>
-      </c>
-      <c r="C6">
-        <f t="shared" ref="C6:AG6" si="1">B6</f>
-        <v>0.99</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="R6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="S6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="T6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="U6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="V6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="W6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="X6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="Y6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="Z6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="AA6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="AB6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="AC6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="AD6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="AE6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="AF6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-      <c r="AG6">
-        <f t="shared" si="1"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+        <v>3.5</v>
+      </c>
+      <c r="C6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="D6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="E6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="F6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="G6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="H6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="I6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="J6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="K6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="L6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="M6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="N6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="O6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="P6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="R6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="S6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="T6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="U6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="V6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="W6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="X6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="Y6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="Z6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AA6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AB6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AC6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AD6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AE6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AF6" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="AG6" s="10">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1462,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1563,7 +1435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>

</xml_diff>